<commit_message>
Puede generar alumnos a partir de un excel de seneca
</commit_message>
<xml_diff>
--- a/web/uploads/test.xlsx
+++ b/web/uploads/test.xlsx
@@ -20,66 +20,78 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="25">
-  <si>
-    <t xml:space="preserve">codigo</t>
-  </si>
-  <si>
-    <t xml:space="preserve">nombre</t>
-  </si>
-  <si>
-    <t xml:space="preserve">apellidos</t>
-  </si>
-  <si>
-    <t xml:space="preserve">fech_nac</t>
-  </si>
-  <si>
-    <t xml:space="preserve">nom_padre</t>
-  </si>
-  <si>
-    <t xml:space="preserve">nom_madre</t>
-  </si>
-  <si>
-    <t xml:space="preserve">A123</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="32">
+  <si>
+    <t xml:space="preserve">Nº Id. Escolar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nombre</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Primer Apellido</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Segundo Apellido</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fecha de nacimiento</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DNI/Pasaporte Primer tutor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DNI/Pasaporte Segundo tutor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Unidad</t>
   </si>
   <si>
     <t xml:space="preserve">Pepe</t>
   </si>
   <si>
-    <t xml:space="preserve">Pérez Ramírez</t>
+    <t xml:space="preserve">Pérez</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ramírez</t>
   </si>
   <si>
     <t xml:space="preserve">1996/01/02</t>
   </si>
   <si>
+    <t xml:space="preserve">12345678A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">12345678F</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4º ESO</t>
+  </si>
+  <si>
     <t xml:space="preserve">Juan</t>
   </si>
   <si>
-    <t xml:space="preserve">Juana</t>
-  </si>
-  <si>
-    <t xml:space="preserve">B234</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ramírez Pérez</t>
+    <t xml:space="preserve"> Pérez</t>
+  </si>
+  <si>
+    <t xml:space="preserve">23456789B</t>
+  </si>
+  <si>
+    <t xml:space="preserve">23456789G</t>
   </si>
   <si>
     <t xml:space="preserve">Pedro</t>
   </si>
   <si>
-    <t xml:space="preserve">Alexa</t>
-  </si>
-  <si>
-    <t xml:space="preserve">C345</t>
-  </si>
-  <si>
-    <t xml:space="preserve">de la rosa romero</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Paca</t>
-  </si>
-  <si>
-    <t xml:space="preserve">D456</t>
+    <t xml:space="preserve">de la rosa</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> romero</t>
+  </si>
+  <si>
+    <t xml:space="preserve">34567891C</t>
+  </si>
+  <si>
+    <t xml:space="preserve">34567891H</t>
   </si>
   <si>
     <t xml:space="preserve">Maria</t>
@@ -88,13 +100,22 @@
     <t xml:space="preserve">Magdalena</t>
   </si>
   <si>
-    <t xml:space="preserve">E567</t>
+    <t xml:space="preserve">45678912D</t>
+  </si>
+  <si>
+    <t xml:space="preserve">45678912I</t>
   </si>
   <si>
     <t xml:space="preserve">Ana</t>
   </si>
   <si>
     <t xml:space="preserve">Annia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">56789123E</t>
+  </si>
+  <si>
+    <t xml:space="preserve">56789123J</t>
   </si>
 </sst>
 </file>
@@ -196,19 +217,22 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H6" activeCellId="0" sqref="H6"/>
+      <selection pane="topLeft" activeCell="E12" activeCellId="0" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="15.2551020408163"/>
-    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="10.4591836734694"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="11.015306122449"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="12.6887755102041"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="15.1173469387755"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="15.2551020408163"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="18.2244897959184"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="23.0816326530612"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="24.8367346938776"/>
+    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -230,105 +254,135 @@
       <c r="F1" s="0" t="s">
         <v>5</v>
       </c>
+      <c r="G1" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="0" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
-        <v>6</v>
+      <c r="A2" s="0" t="n">
+        <v>1234567</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="D2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E2" s="0" t="s">
+      <c r="D2" s="0" t="s">
         <v>10</v>
       </c>
+      <c r="E2" s="1" t="s">
+        <v>11</v>
+      </c>
       <c r="F2" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
+      </c>
+      <c r="G2" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="H2" s="0" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
-        <v>12</v>
+      <c r="A3" s="0" t="n">
+        <v>2345678</v>
       </c>
       <c r="B3" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" s="0" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E3" s="0" t="s">
-        <v>14</v>
+      <c r="D3" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>11</v>
       </c>
       <c r="F3" s="0" t="s">
-        <v>15</v>
+        <v>17</v>
+      </c>
+      <c r="G3" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="H3" s="0" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
-        <v>16</v>
+      <c r="A4" s="0" t="n">
+        <v>3456789</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E4" s="0" t="s">
-        <v>7</v>
+        <v>20</v>
+      </c>
+      <c r="D4" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>11</v>
       </c>
       <c r="F4" s="0" t="s">
-        <v>18</v>
+        <v>22</v>
+      </c>
+      <c r="G4" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="H4" s="0" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
-        <v>19</v>
+      <c r="A5" s="0" t="n">
+        <v>4567891</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E5" s="0" t="s">
-        <v>10</v>
+        <v>25</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>11</v>
       </c>
       <c r="F5" s="0" t="s">
-        <v>18</v>
+        <v>26</v>
+      </c>
+      <c r="G5" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="H5" s="0" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
-        <v>22</v>
+      <c r="A6" s="0" t="n">
+        <v>5678912</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E6" s="0" t="s">
-        <v>7</v>
+        <v>29</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>11</v>
       </c>
       <c r="F6" s="0" t="s">
-        <v>20</v>
+        <v>30</v>
+      </c>
+      <c r="G6" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="H6" s="0" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Decimos que campos queremos y si no mandamos error
</commit_message>
<xml_diff>
--- a/web/uploads/test.xlsx
+++ b/web/uploads/test.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="27">
   <si>
     <t xml:space="preserve">Nº Id. Escolar</t>
   </si>
@@ -28,9 +28,6 @@
     <t xml:space="preserve">Nombre</t>
   </si>
   <si>
-    <t xml:space="preserve">Primer Apellido</t>
-  </si>
-  <si>
     <t xml:space="preserve">Segundo Apellido</t>
   </si>
   <si>
@@ -49,9 +46,6 @@
     <t xml:space="preserve">Pepe</t>
   </si>
   <si>
-    <t xml:space="preserve">Pérez</t>
-  </si>
-  <si>
     <t xml:space="preserve">Ramírez</t>
   </si>
   <si>
@@ -82,9 +76,6 @@
     <t xml:space="preserve">Pedro</t>
   </si>
   <si>
-    <t xml:space="preserve">de la rosa</t>
-  </si>
-  <si>
     <t xml:space="preserve"> romero</t>
   </si>
   <si>
@@ -97,9 +88,6 @@
     <t xml:space="preserve">Maria</t>
   </si>
   <si>
-    <t xml:space="preserve">Magdalena</t>
-  </si>
-  <si>
     <t xml:space="preserve">45678912D</t>
   </si>
   <si>
@@ -107,9 +95,6 @@
   </si>
   <si>
     <t xml:space="preserve">Ana</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Annia</t>
   </si>
   <si>
     <t xml:space="preserve">56789123E</t>
@@ -220,19 +205,17 @@
   <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E12" activeCellId="0" sqref="E12"/>
+      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1:C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="12.6887755102041"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="15.1173469387755"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="15.2551020408163"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="18.2244897959184"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="23.0816326530612"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="24.8367346938776"/>
-    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="12.4183673469388"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="14.5816326530612"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="14.8469387755102"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="17.8214285714286"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="22.5459183673469"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="24.3010204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -242,23 +225,20 @@
       <c r="B1" s="0" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="D1" s="0" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="0" t="s">
+      <c r="E1" s="0" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="0" t="s">
+      <c r="F1" s="0" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="0" t="s">
+      <c r="G1" s="0" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="0" t="s">
+      <c r="H1" s="0" t="s">
         <v>6</v>
-      </c>
-      <c r="H1" s="0" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -266,25 +246,22 @@
         <v>1234567</v>
       </c>
       <c r="B2" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="D2" s="0" t="s">
+      <c r="E2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F2" s="0" t="s">
         <v>10</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="G2" s="0" t="s">
         <v>11</v>
       </c>
-      <c r="F2" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="G2" s="0" t="s">
-        <v>13</v>
-      </c>
       <c r="H2" s="0" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -292,25 +269,22 @@
         <v>2345678</v>
       </c>
       <c r="B3" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F3" s="0" t="s">
         <v>15</v>
       </c>
-      <c r="C3" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="D3" s="0" t="s">
+      <c r="G3" s="0" t="s">
         <v>16</v>
       </c>
-      <c r="E3" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="F3" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="G3" s="0" t="s">
-        <v>18</v>
-      </c>
       <c r="H3" s="0" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -318,25 +292,22 @@
         <v>3456789</v>
       </c>
       <c r="B4" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="D4" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F4" s="0" t="s">
         <v>19</v>
       </c>
-      <c r="C4" s="0" t="s">
+      <c r="G4" s="0" t="s">
         <v>20</v>
       </c>
-      <c r="D4" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="F4" s="0" t="s">
-        <v>22</v>
-      </c>
-      <c r="G4" s="0" t="s">
-        <v>23</v>
-      </c>
       <c r="H4" s="0" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -344,22 +315,19 @@
         <v>4567891</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="C5" s="0" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="F5" s="0" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="G5" s="0" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="H5" s="0" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -367,22 +335,19 @@
         <v>5678912</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>28</v>
-      </c>
-      <c r="C6" s="0" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="F6" s="0" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="G6" s="0" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="H6" s="0" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
cambiamos un poco el diseño de la pagina y modificamos el index
</commit_message>
<xml_diff>
--- a/web/uploads/test.xlsx
+++ b/web/uploads/test.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="32">
   <si>
     <t xml:space="preserve">Nº Id. Escolar</t>
   </si>
@@ -28,6 +28,9 @@
     <t xml:space="preserve">Nombre</t>
   </si>
   <si>
+    <t xml:space="preserve">Primer Apellido</t>
+  </si>
+  <si>
     <t xml:space="preserve">Segundo Apellido</t>
   </si>
   <si>
@@ -46,6 +49,9 @@
     <t xml:space="preserve">Pepe</t>
   </si>
   <si>
+    <t xml:space="preserve">Pérez</t>
+  </si>
+  <si>
     <t xml:space="preserve">Ramírez</t>
   </si>
   <si>
@@ -76,6 +82,9 @@
     <t xml:space="preserve">Pedro</t>
   </si>
   <si>
+    <t xml:space="preserve">de la rosa</t>
+  </si>
+  <si>
     <t xml:space="preserve"> romero</t>
   </si>
   <si>
@@ -88,6 +97,9 @@
     <t xml:space="preserve">Maria</t>
   </si>
   <si>
+    <t xml:space="preserve">Magdalena</t>
+  </si>
+  <si>
     <t xml:space="preserve">45678912D</t>
   </si>
   <si>
@@ -95,6 +107,9 @@
   </si>
   <si>
     <t xml:space="preserve">Ana</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Annia</t>
   </si>
   <si>
     <t xml:space="preserve">56789123E</t>
@@ -225,20 +240,23 @@
       <c r="B1" s="0" t="s">
         <v>1</v>
       </c>
+      <c r="C1" s="0" t="s">
+        <v>2</v>
+      </c>
       <c r="D1" s="0" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H1" s="0" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -246,22 +264,25 @@
         <v>1234567</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>7</v>
+        <v>8</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>9</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="G2" s="0" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="H2" s="0" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -269,22 +290,25 @@
         <v>2345678</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>13</v>
+        <v>15</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>10</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="F3" s="0" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="G3" s="0" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="H3" s="0" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -292,22 +316,25 @@
         <v>3456789</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>17</v>
+        <v>19</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>20</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="F4" s="0" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="G4" s="0" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="H4" s="0" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -315,19 +342,22 @@
         <v>4567891</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>21</v>
+        <v>24</v>
+      </c>
+      <c r="C5" s="0" t="s">
+        <v>25</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="F5" s="0" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="G5" s="0" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="H5" s="0" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -335,19 +365,22 @@
         <v>5678912</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>24</v>
+        <v>28</v>
+      </c>
+      <c r="C6" s="0" t="s">
+        <v>29</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="F6" s="0" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="G6" s="0" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="H6" s="0" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
arreglos carga archivo alumnos y envio de correos
</commit_message>
<xml_diff>
--- a/web/uploads/test.xlsx
+++ b/web/uploads/test.xlsx
@@ -220,17 +220,19 @@
   <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1:C6"/>
+      <selection pane="topLeft" activeCell="F13" activeCellId="0" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="12.4183673469388"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="14.5816326530612"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="14.8469387755102"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="17.8214285714286"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="22.5459183673469"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="24.3010204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="12.1479591836735"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="14.0408163265306"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="15.4591836734694"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="17.280612244898"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="23.3826530612245"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="25.1887755102041"/>
+    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>